<commit_message>
Moved script & doc from pos-mobile repository
</commit_message>
<xml_diff>
--- a/Evolution of tables.xlsx
+++ b/Evolution of tables.xlsx
@@ -32,33 +32,41 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Some tables are dropped</t>
-  </si>
-  <si>
     <t>Columns are retyped.</t>
   </si>
   <si>
-    <t>Some columns are dropped.</t>
-  </si>
-  <si>
-    <t>Some columns are renamed.</t>
-  </si>
-  <si>
-    <t>Some tables are renamed.</t>
-  </si>
-  <si>
-    <t>Some tables are ignored (not described) in Excel workbooks for version 1A.</t>
-  </si>
-  <si>
-    <t>Some columns are changed from mandatory to optional. Two tables renamed. Tickets and TicketLines. Products_kit and Products_com are unused.</t>
+    <t>Some tables are added and/or renamed (e.g, Product_kits; with different name).</t>
+  </si>
+  <si>
+    <t>Some columns are changed from mandatory to optional. Two tables renamed. Tickets and TicketLines. Some tables are dropped. More constraints are dropped.</t>
+  </si>
+  <si>
+    <t>Some tables are ignored (not described) in Excel workbooks for version 1A. Some constraints are dropped.</t>
+  </si>
+  <si>
+    <t>Some columns are dropped: SFlag, SiteGUId, Attribute*.</t>
+  </si>
+  <si>
+    <t>Some columns are renamed (and merged [name]). Some constraints are renamed</t>
+  </si>
+  <si>
+    <t>Some tables are renamed (including Products_*). Some relationships are changed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -110,6 +118,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,29 +402,29 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.109375" customWidth="1"/>
+    <col min="2" max="2" width="67.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -423,7 +432,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -431,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -439,7 +448,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -447,7 +456,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -455,7 +464,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -463,7 +472,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>